<commit_message>
data-all file with more data
</commit_message>
<xml_diff>
--- a/data/data-all.xlsx
+++ b/data/data-all.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konark\Documents\360 Proj\CISC360-Project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konark\Documents\360 Project\CISC360-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18735" windowHeight="7965" activeTab="1" xr2:uid="{69A3D522-E722-4A7B-8B0B-58C35D2C7C0D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18735" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="ICG" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="50">
   <si>
     <t>XORSHIFT: ADVANCED HOTSPOTS AVG</t>
   </si>
@@ -175,12 +175,15 @@
   </si>
   <si>
     <t>Average Latency (cycles):</t>
+  </si>
+  <si>
+    <t>Mike</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -273,7 +276,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -584,11 +587,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17237CB7-1AED-43F9-ADBB-8BF666B4AA14}">
-  <dimension ref="A1:G28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -596,15 +599,16 @@
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
@@ -615,8 +619,11 @@
       <c r="F2" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -638,8 +645,14 @@
       <c r="G3" s="19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>240.553</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
@@ -661,8 +674,14 @@
       <c r="G4" s="19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>237.03200000000001</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
@@ -677,8 +696,11 @@
         <v>673506692379</v>
       </c>
       <c r="G5" s="18"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>437203886404.38568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
@@ -693,8 +715,11 @@
         <v>5361147313.666667</v>
       </c>
       <c r="G6" s="18"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>106363382318.33333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
@@ -709,8 +734,11 @@
         <v>1.554</v>
       </c>
       <c r="G7" s="18"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>62116363435.800331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="17" t="s">
         <v>37</v>
       </c>
@@ -718,8 +746,11 @@
         <v>0</v>
       </c>
       <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="6" t="s">
         <v>22</v>
       </c>
@@ -734,8 +765,11 @@
         <v>1.1166666666666669</v>
       </c>
       <c r="G9" s="18"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9">
+        <v>11.758666666666665</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="17" t="s">
         <v>38</v>
       </c>
@@ -745,8 +779,14 @@
       <c r="G10" s="19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10">
+        <v>0.36266666666666669</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="6" t="s">
         <v>20</v>
       </c>
@@ -761,8 +801,11 @@
         <v>5361147313.666667</v>
       </c>
       <c r="G11" s="18"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11">
+        <v>3023015533.6666665</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -777,8 +820,11 @@
         <v>1</v>
       </c>
       <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -800,19 +846,25 @@
       <c r="G13" s="19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" s="4" t="s">
         <v>1</v>
       </c>
@@ -828,10 +880,20 @@
       <c r="E16" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="F16" s="19">
+        <v>281.5333333333333</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16">
+        <v>235.19033333333334</v>
+      </c>
+      <c r="I16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="4" t="s">
         <v>2</v>
       </c>
@@ -848,13 +910,19 @@
         <v>17</v>
       </c>
       <c r="F17" s="19">
-        <v>281.5333333333333</v>
+        <v>197.73733333333334</v>
       </c>
       <c r="G17" s="19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17">
+        <v>173.99</v>
+      </c>
+      <c r="I17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
@@ -865,14 +933,11 @@
       <c r="D18">
         <v>0.19666666666666668</v>
       </c>
-      <c r="F18" s="19">
-        <v>197.73733333333334</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
@@ -883,7 +948,7 @@
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:9">
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
@@ -896,7 +961,7 @@
       </c>
       <c r="G20" s="18"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:9">
       <c r="A21" s="4" t="s">
         <v>28</v>
       </c>
@@ -909,7 +974,7 @@
       </c>
       <c r="G21" s="18"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:9">
       <c r="A22" s="4" t="s">
         <v>29</v>
       </c>
@@ -922,7 +987,7 @@
       </c>
       <c r="G22" s="18"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:9">
       <c r="A23" s="4" t="s">
         <v>11</v>
       </c>
@@ -937,8 +1002,11 @@
         <v>222999689790</v>
       </c>
       <c r="G23" s="18"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23">
+        <v>229353947078.66666</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="4" t="s">
         <v>12</v>
       </c>
@@ -953,8 +1021,11 @@
         <v>133943218176</v>
       </c>
       <c r="G24" s="18"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24">
+        <v>137461490387.66666</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
@@ -969,8 +1040,11 @@
         <v>4700141</v>
       </c>
       <c r="G25" s="18"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25">
+        <v>466680.66666666669</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
@@ -985,8 +1059,11 @@
         <v>35</v>
       </c>
       <c r="G26" s="18"/>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26">
+        <v>33.666666666666664</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
@@ -1001,8 +1078,11 @@
         <v>1</v>
       </c>
       <c r="G27" s="18"/>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="4" t="s">
         <v>8</v>
       </c>
@@ -1022,6 +1102,12 @@
         <v>0</v>
       </c>
       <c r="G28" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1032,11 +1118,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D24D3C-9519-485B-AFF3-6D48F96BCCDD}">
-  <dimension ref="A1:G28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1045,14 +1131,15 @@
     <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1063,8 +1150,11 @@
       <c r="F2" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1086,8 +1176,14 @@
       <c r="G3" s="38" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>19.048666666666666</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1109,8 +1205,14 @@
       <c r="G4" s="38" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>17.862666666666666</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -1125,8 +1227,11 @@
         <v>140468017942.33334</v>
       </c>
       <c r="G5" s="37"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>135036961568.66667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -1141,8 +1246,11 @@
         <v>4299523480</v>
       </c>
       <c r="G6" s="37"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>3569555276.6666665</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -1157,14 +1265,20 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="G7" s="37"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>0.4366666666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="F8" s="38">
         <v>0</v>
       </c>
       <c r="G8" s="37"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
@@ -1179,16 +1293,25 @@
         <v>1.0776666666666666</v>
       </c>
       <c r="G9" s="37"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9">
+        <v>1.1386666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="F10" s="38">
         <v>1.5666666666666666E-2</v>
       </c>
       <c r="G10" s="38" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10">
+        <v>0.28166666666666668</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="7" t="s">
         <v>4</v>
       </c>
@@ -1203,8 +1326,11 @@
         <v>4299523480</v>
       </c>
       <c r="G11" s="37"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11">
+        <v>3569555276.6666665</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -1219,8 +1345,11 @@
         <v>1</v>
       </c>
       <c r="G12" s="37"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
@@ -1242,15 +1371,21 @@
       <c r="G13" s="38" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" s="7" t="s">
         <v>1</v>
       </c>
@@ -1266,10 +1401,20 @@
       <c r="E16" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="F16" s="38">
+        <v>19.934333333333331</v>
+      </c>
+      <c r="G16" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16">
+        <v>16.032666666666668</v>
+      </c>
+      <c r="I16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="7" t="s">
         <v>2</v>
       </c>
@@ -1286,13 +1431,19 @@
         <v>17</v>
       </c>
       <c r="F17" s="38">
-        <v>19.934333333333331</v>
+        <v>13.569999999999999</v>
       </c>
       <c r="G17" s="38" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17">
+        <v>15.703333333333333</v>
+      </c>
+      <c r="I17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="7" t="s">
         <v>10</v>
       </c>
@@ -1303,30 +1454,31 @@
       <c r="D18">
         <v>8.8666666666666671E-2</v>
       </c>
-      <c r="F18" s="38">
-        <v>13.569999999999999</v>
-      </c>
-      <c r="G18" s="38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="F19" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18">
+        <v>1.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="F19" s="38">
+        <v>3.6666666666666666E-3</v>
+      </c>
       <c r="G19" s="37"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:9">
       <c r="F20" s="38">
-        <v>3.6666666666666666E-3</v>
+        <v>0</v>
       </c>
       <c r="G20" s="37"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:9">
       <c r="F21" s="38">
-        <v>0</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="G21" s="37"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:9">
       <c r="A22" s="7" t="s">
         <v>11</v>
       </c>
@@ -1338,11 +1490,14 @@
         <v>69876496232</v>
       </c>
       <c r="F22" s="38">
-        <v>3.3333333333333332E-4</v>
+        <v>48941068188</v>
       </c>
       <c r="G22" s="37"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22">
+        <v>66904973755.666664</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="7" t="s">
         <v>12</v>
       </c>
@@ -1354,11 +1509,14 @@
         <v>34923647678</v>
       </c>
       <c r="F23" s="38">
-        <v>48941068188</v>
+        <v>24468934046</v>
       </c>
       <c r="G23" s="37"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23">
+        <v>33439536489.333332</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="7" t="s">
         <v>13</v>
       </c>
@@ -1370,11 +1528,14 @@
         <v>400012</v>
       </c>
       <c r="F24" s="38">
-        <v>24468934046</v>
+        <v>900027</v>
       </c>
       <c r="G24" s="37"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24">
+        <v>466680.66666666669</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="7" t="s">
         <v>14</v>
       </c>
@@ -1386,11 +1547,14 @@
         <v>9</v>
       </c>
       <c r="F25" s="38">
-        <v>900027</v>
+        <v>10</v>
       </c>
       <c r="G25" s="37"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25">
+        <v>10.666666666666666</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="7" t="s">
         <v>7</v>
       </c>
@@ -1402,11 +1566,14 @@
         <v>1</v>
       </c>
       <c r="F26" s="38">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G26" s="37"/>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="7" t="s">
         <v>8</v>
       </c>
@@ -1423,29 +1590,30 @@
         <v>17</v>
       </c>
       <c r="F27" s="38">
-        <v>1</v>
-      </c>
-      <c r="G27" s="37"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="F28" s="38">
-        <v>0</v>
-      </c>
-      <c r="G28" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FD1DFC-03B8-497F-8D2C-86FF3F62A726}">
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1454,9 +1622,10 @@
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1467,13 +1636,16 @@
       <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
@@ -1495,8 +1667,14 @@
       <c r="G3" s="33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>235.88533333333336</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="31" t="s">
         <v>18</v>
       </c>
@@ -1518,8 +1696,14 @@
       <c r="G4" s="33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>229.31833333333336</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="31" t="s">
         <v>19</v>
       </c>
@@ -1534,8 +1718,11 @@
         <v>1635863940831</v>
       </c>
       <c r="G5" s="32"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>1610462702156.3333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="31" t="s">
         <v>20</v>
       </c>
@@ -1550,8 +1737,11 @@
         <v>4448130921</v>
       </c>
       <c r="G6" s="32"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>4270867086</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="31" t="s">
         <v>21</v>
       </c>
@@ -1566,8 +1756,11 @@
         <v>0.5093333333333333</v>
       </c>
       <c r="G7" s="32"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="31" t="s">
         <v>39</v>
       </c>
@@ -1575,8 +1768,11 @@
         <v>0</v>
       </c>
       <c r="G8" s="32"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="31" t="s">
         <v>22</v>
       </c>
@@ -1591,8 +1787,11 @@
         <v>1.0860000000000001</v>
       </c>
       <c r="G9" s="32"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9">
+        <v>1.1379999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="31" t="s">
         <v>40</v>
       </c>
@@ -1602,8 +1801,14 @@
       <c r="G10" s="33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10">
+        <v>0.19333333333333333</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="31" t="s">
         <v>20</v>
       </c>
@@ -1618,8 +1823,11 @@
         <v>4448130921</v>
       </c>
       <c r="G11" s="32"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11">
+        <v>4270867086</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="31" t="s">
         <v>23</v>
       </c>
@@ -1634,8 +1842,11 @@
         <v>1</v>
       </c>
       <c r="G12" s="32"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="31" t="s">
         <v>24</v>
       </c>
@@ -1657,15 +1868,21 @@
       <c r="G13" s="33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" s="34" t="s">
         <v>1</v>
       </c>
@@ -1687,8 +1904,14 @@
       <c r="G16" s="36" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16">
+        <v>228.36766666666668</v>
+      </c>
+      <c r="I16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="34" t="s">
         <v>18</v>
       </c>
@@ -1710,8 +1933,14 @@
       <c r="G17" s="36" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17">
+        <v>165.31700000000001</v>
+      </c>
+      <c r="I17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="34" t="s">
         <v>44</v>
       </c>
@@ -1724,8 +1953,11 @@
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="35"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18">
+        <v>2.0666666666666667E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="34" t="s">
         <v>41</v>
       </c>
@@ -1734,7 +1966,7 @@
       </c>
       <c r="G19" s="35"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:9">
       <c r="A20" s="34" t="s">
         <v>42</v>
       </c>
@@ -1743,7 +1975,7 @@
       </c>
       <c r="G20" s="35"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:9">
       <c r="A21" s="34" t="s">
         <v>43</v>
       </c>
@@ -1752,7 +1984,7 @@
       </c>
       <c r="G21" s="35"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:9">
       <c r="A22" s="34" t="s">
         <v>45</v>
       </c>
@@ -1767,8 +1999,11 @@
         <v>745130953258</v>
       </c>
       <c r="G22" s="35"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22">
+        <v>543846548240.33301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="34" t="s">
         <v>46</v>
       </c>
@@ -1783,8 +2018,11 @@
         <v>186617898369</v>
       </c>
       <c r="G23" s="35"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23">
+        <v>136093182673</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="34" t="s">
         <v>47</v>
       </c>
@@ -1799,8 +2037,11 @@
         <v>12000360</v>
       </c>
       <c r="G24" s="35"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24">
+        <v>933361.33333333337</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="34" t="s">
         <v>48</v>
       </c>
@@ -1815,8 +2056,11 @@
         <v>10</v>
       </c>
       <c r="G25" s="35"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="34" t="s">
         <v>23</v>
       </c>
@@ -1831,8 +2075,11 @@
         <v>1</v>
       </c>
       <c r="G26" s="35"/>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="34" t="s">
         <v>24</v>
       </c>
@@ -1852,6 +2099,12 @@
         <v>0</v>
       </c>
       <c r="G27" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1861,11 +2114,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395873E2-967B-44E6-BE22-7E6E73DA4430}">
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1874,14 +2127,15 @@
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1892,8 +2146,11 @@
       <c r="F2" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
@@ -1915,8 +2172,14 @@
       <c r="G3" s="27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>56.728333333333332</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="27" t="s">
         <v>18</v>
       </c>
@@ -1938,8 +2201,14 @@
       <c r="G4" s="27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>53.552999999999997</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="27" t="s">
         <v>19</v>
       </c>
@@ -1954,8 +2223,11 @@
         <v>321009809158.33331</v>
       </c>
       <c r="G5" s="26"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>310941554862</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="27" t="s">
         <v>20</v>
       </c>
@@ -1970,8 +2242,11 @@
         <v>8486348528.666667</v>
       </c>
       <c r="G6" s="26"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>8519563893.333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="27" t="s">
         <v>21</v>
       </c>
@@ -1986,8 +2261,11 @@
         <v>0.69499999999999995</v>
       </c>
       <c r="G7" s="26"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>0.56800000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="27" t="s">
         <v>39</v>
       </c>
@@ -1995,8 +2273,11 @@
         <v>0</v>
       </c>
       <c r="G8" s="26"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="27" t="s">
         <v>22</v>
       </c>
@@ -2011,8 +2292,11 @@
         <v>1.0803333333333334</v>
       </c>
       <c r="G9" s="26"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9">
+        <v>1.1373333333333333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="27" t="s">
         <v>40</v>
       </c>
@@ -2022,8 +2306,14 @@
       <c r="G10" s="27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10">
+        <v>0.16566666666666666</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="27" t="s">
         <v>20</v>
       </c>
@@ -2038,8 +2328,11 @@
         <v>8486348528.666667</v>
       </c>
       <c r="G11" s="26"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11">
+        <v>8519563893.333333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="27" t="s">
         <v>23</v>
       </c>
@@ -2054,8 +2347,11 @@
         <v>1</v>
       </c>
       <c r="G12" s="26"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="27" t="s">
         <v>24</v>
       </c>
@@ -2077,15 +2373,21 @@
       <c r="G13" s="27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="13" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" s="30" t="s">
         <v>1</v>
       </c>
@@ -2107,8 +2409,14 @@
       <c r="G16" s="29" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16">
+        <v>50.339666666666666</v>
+      </c>
+      <c r="I16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="30" t="s">
         <v>18</v>
       </c>
@@ -2130,8 +2438,14 @@
       <c r="G17" s="29" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17">
+        <v>49.746333333333332</v>
+      </c>
+      <c r="I17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="30" t="s">
         <v>44</v>
       </c>
@@ -2144,8 +2458,11 @@
       </c>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18">
+        <v>1.5333333333333332E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="30" t="s">
         <v>41</v>
       </c>
@@ -2154,7 +2471,7 @@
       </c>
       <c r="G19" s="28"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:9">
       <c r="A20" s="30" t="s">
         <v>42</v>
       </c>
@@ -2163,7 +2480,7 @@
       </c>
       <c r="G20" s="28"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:9">
       <c r="A21" s="30" t="s">
         <v>43</v>
       </c>
@@ -2172,7 +2489,7 @@
       </c>
       <c r="G21" s="28"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:9">
       <c r="A22" s="30" t="s">
         <v>45</v>
       </c>
@@ -2187,8 +2504,11 @@
         <v>94211426258</v>
       </c>
       <c r="G22" s="28"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22">
+        <v>93709011186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="30" t="s">
         <v>46</v>
       </c>
@@ -2203,8 +2523,11 @@
         <v>55666769953</v>
       </c>
       <c r="G23" s="28"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23">
+        <v>55358827381.666664</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="30" t="s">
         <v>47</v>
       </c>
@@ -2219,8 +2542,11 @@
         <v>3200096</v>
       </c>
       <c r="G24" s="28"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="30" t="s">
         <v>48</v>
       </c>
@@ -2235,8 +2561,11 @@
         <v>15</v>
       </c>
       <c r="G25" s="28"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25">
+        <v>14.333333333333334</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="30" t="s">
         <v>23</v>
       </c>
@@ -2251,8 +2580,11 @@
         <v>1</v>
       </c>
       <c r="G26" s="28"/>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="30" t="s">
         <v>24</v>
       </c>
@@ -2272,6 +2604,12 @@
         <v>0</v>
       </c>
       <c r="G27" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2281,11 +2619,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAF2C974-C46E-41CA-9E83-1379BED171A6}">
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2294,9 +2632,10 @@
     <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2307,13 +2646,16 @@
       <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
@@ -2335,8 +2677,14 @@
       <c r="G3" s="22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="14">
+        <v>35.596666666666671</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
@@ -2358,8 +2706,14 @@
       <c r="G4" s="22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="14">
+        <v>34.204333333333331</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="20" t="s">
         <v>19</v>
       </c>
@@ -2374,8 +2728,12 @@
         <v>239975302192.33334</v>
       </c>
       <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="14">
+        <v>234597014946.66666</v>
+      </c>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="20" t="s">
         <v>20</v>
       </c>
@@ -2390,8 +2748,12 @@
         <v>4320201945.333333</v>
       </c>
       <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="14">
+        <v>4263225018.6666665</v>
+      </c>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="20" t="s">
         <v>21</v>
       </c>
@@ -2406,8 +2768,12 @@
         <v>0.57933333333333337</v>
       </c>
       <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="14">
+        <v>0.48100000000000004</v>
+      </c>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="20" t="s">
         <v>39</v>
       </c>
@@ -2415,8 +2781,12 @@
         <v>0</v>
       </c>
       <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="14">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="20" t="s">
         <v>22</v>
       </c>
@@ -2431,8 +2801,12 @@
         <v>1.1196666666666666</v>
       </c>
       <c r="G9" s="21"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="14">
+        <v>1.1369999999999998</v>
+      </c>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="20" t="s">
         <v>40</v>
       </c>
@@ -2442,8 +2816,14 @@
       <c r="G10" s="22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="14">
+        <v>0.31566666666666671</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="20" t="s">
         <v>20</v>
       </c>
@@ -2458,8 +2838,12 @@
         <v>4320201945.333333</v>
       </c>
       <c r="G11" s="21"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="14">
+        <v>4263225018.6666665</v>
+      </c>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="20" t="s">
         <v>23</v>
       </c>
@@ -2474,8 +2858,12 @@
         <v>1</v>
       </c>
       <c r="G12" s="21"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="14">
+        <v>1</v>
+      </c>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="20" t="s">
         <v>24</v>
       </c>
@@ -2497,15 +2885,21 @@
       <c r="G13" s="22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H13" s="14">
+        <v>0</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" s="14" t="s">
         <v>1</v>
       </c>
@@ -2527,8 +2921,14 @@
       <c r="G16" s="24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16">
+        <v>34.673999999999999</v>
+      </c>
+      <c r="I16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="14" t="s">
         <v>2</v>
       </c>
@@ -2550,8 +2950,14 @@
       <c r="G17" s="24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17">
+        <v>34.009666666666668</v>
+      </c>
+      <c r="I17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="14" t="s">
         <v>10</v>
       </c>
@@ -2564,8 +2970,11 @@
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18">
+        <v>2.1666666666666667E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="25" t="s">
         <v>41</v>
       </c>
@@ -2574,7 +2983,7 @@
       </c>
       <c r="G19" s="23"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:9">
       <c r="A20" s="25" t="s">
         <v>42</v>
       </c>
@@ -2583,7 +2992,7 @@
       </c>
       <c r="G20" s="23"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:9">
       <c r="A21" s="25" t="s">
         <v>43</v>
       </c>
@@ -2592,7 +3001,7 @@
       </c>
       <c r="G21" s="23"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:9">
       <c r="A22" s="14" t="s">
         <v>11</v>
       </c>
@@ -2607,8 +3016,11 @@
         <v>117228616753</v>
       </c>
       <c r="G22" s="23"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22">
+        <v>118739195402.33333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="14" t="s">
         <v>12</v>
       </c>
@@ -2623,8 +3035,11 @@
         <v>41900156967</v>
       </c>
       <c r="G23" s="23"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23">
+        <v>42413339028.666664</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="14" t="s">
         <v>13</v>
       </c>
@@ -2639,8 +3054,11 @@
         <v>1500045</v>
       </c>
       <c r="G24" s="23"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24">
+        <v>233340.33333333334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="14" t="s">
         <v>14</v>
       </c>
@@ -2655,8 +3073,11 @@
         <v>13.333333333333334</v>
       </c>
       <c r="G25" s="23"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25">
+        <v>15.666666666666666</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="14" t="s">
         <v>7</v>
       </c>
@@ -2671,8 +3092,11 @@
         <v>1</v>
       </c>
       <c r="G26" s="23"/>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="14" t="s">
         <v>8</v>
       </c>
@@ -2692,6 +3116,12 @@
         <v>0</v>
       </c>
       <c r="G27" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>